<commit_message>
Se actualizan los costos de los componentes
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7B9AA2-4788-4FF6-8794-EDE5CCAC0A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FCBFE5-D719-4567-8C14-D622DEBE667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>COMPONENTE</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Pressure</t>
   </si>
   <si>
-    <t>Transceiver</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -154,6 +151,24 @@
   </si>
   <si>
     <t>Voltage regulator 3.3V</t>
+  </si>
+  <si>
+    <t>Air quality</t>
+  </si>
+  <si>
+    <t>MQ-7</t>
+  </si>
+  <si>
+    <t>UNIT - MQ7</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>40 Pins 2mm</t>
+  </si>
+  <si>
+    <t>UNIT - Headers</t>
   </si>
 </sst>
 </file>
@@ -215,7 +230,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,6 +247,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -552,7 +570,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,14 +621,14 @@
         <v>27</v>
       </c>
       <c r="D2" s="3">
-        <v>45.69</v>
+        <v>114</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3">
         <f>D2*E2</f>
-        <v>45.69</v>
+        <v>228</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -657,14 +675,14 @@
         <v>28</v>
       </c>
       <c r="D4" s="3">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
@@ -732,18 +750,34 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="F7" s="3">
         <f t="shared" ref="F7:F8" si="1">D7*E7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -773,7 +807,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
@@ -801,21 +835,21 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
-        <v>4.3099999999999996</v>
+        <v>23</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ref="F10" si="3">D10*E10</f>
-        <v>4.3099999999999996</v>
+        <f t="shared" ref="F10:F11" si="3">D10*E10</f>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>11</v>
@@ -828,7 +862,32 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C11" s="3"/>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
@@ -905,13 +964,32 @@
     <hyperlink ref="I4" r:id="rId14" xr:uid="{B1E876DB-7A87-4E4B-BF53-D9DA749148B8}"/>
     <hyperlink ref="I3" r:id="rId15" xr:uid="{A0132019-F399-4A59-9165-71A7CDAAFE35}"/>
     <hyperlink ref="I2" r:id="rId16" xr:uid="{16A86D44-50E5-4F3A-9961-5FEB35DC0B59}"/>
+    <hyperlink ref="H7" r:id="rId17" xr:uid="{30C3594F-83B1-4803-92BF-7DDC3E755E7B}"/>
+    <hyperlink ref="I7" r:id="rId18" xr:uid="{590A9D43-B89D-445C-B143-A8B9100990D9}"/>
+    <hyperlink ref="H11" r:id="rId19" xr:uid="{A467FD39-2555-4C04-B90D-1A58A1E55DEA}"/>
+    <hyperlink ref="I11" r:id="rId20" xr:uid="{B81C7B8D-AEA0-4586-AB45-139637A8ECCE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010009B1883D8FF5A14C94F242EAFB7A34AC" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f7fd207d1d9afdcbfae569e1434e011">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bce897b7-2960-4354-a964-18cb830148f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02997fdaf8a2097aeb6b595533e4c626" ns2:_="">
     <xsd:import namespace="bce897b7-2960-4354-a964-18cb830148f8"/>
@@ -1049,35 +1127,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC9FCAA-3BFA-488C-952F-8BCEDC98A4B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16621656-C4AE-4B29-96FF-2168302B9EFE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bce897b7-2960-4354-a964-18cb830148f8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1099,9 +1152,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16621656-C4AE-4B29-96FF-2168302B9EFE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC9FCAA-3BFA-488C-952F-8BCEDC98A4B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bce897b7-2960-4354-a964-18cb830148f8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>